<commit_message>
Update HW8 with new plotting instructions
because Plotly no longer allows new accounts
</commit_message>
<xml_diff>
--- a/Lectures/Ex2-1Dual.xlsx
+++ b/Lectures/Ex2-1Dual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Box\_Rosenberg2024\Classes\CEE6410\Fall2024\CEE6410-Rosenberg-GitHub\CEE-6410-Rosenberg\Lectures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF6BF24F-29C0-4CFC-BF37-5DE39FC96B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F18F206-8268-402C-8C82-7A0E8CC975DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7270" xr2:uid="{BFE000EE-E438-4CD7-B8D4-56F26CA06FA6}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" xr2:uid="{55395D80-39AC-451B-A160-2F09F4DD3438}"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="11" r:id="rId1"/>
@@ -604,7 +604,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1228CD-7029-4A6B-AF33-0DBBF7766C0A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32FFAB76-4932-4993-B56F-965F4B099A6A}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -851,26 +851,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" location="A!A1" display="A" xr:uid="{7E9689C7-813D-415C-8807-A742734D9EE2}"/>
-    <hyperlink ref="A3" location="b!A1" display="b" xr:uid="{7D8EAB90-9E6C-46A5-A024-705F755C79F4}"/>
-    <hyperlink ref="A4" location="c!A1" display="c" xr:uid="{D5DCD090-37F0-4515-8437-6390C2ADA24B}"/>
-    <hyperlink ref="A5" location="plnt!A1" display="plnt" xr:uid="{6621AA4A-CD70-42D2-89E0-1D018089A7CA}"/>
-    <hyperlink ref="A6" location="Scalar!A1" display="PROFIT_PRIMAL" xr:uid="{F6DF91D2-A263-4742-8976-D94DF3CC29D0}"/>
-    <hyperlink ref="A7" location="Scalar!A1" display="REDCOST_DUAL" xr:uid="{344431F9-7369-4FDD-B5F9-FB86219E4F9A}"/>
-    <hyperlink ref="A8" location="res!A1" display="res" xr:uid="{92AE4DD0-BCB5-4920-AF2F-B31AF5D6793D}"/>
-    <hyperlink ref="A9" location="RES_CONS_DUAL!A1" display="RES_CONS_DUAL" xr:uid="{BF21EED4-8D33-4D6F-AE87-A67F137AEF98}"/>
-    <hyperlink ref="A10" location="RES_CONS_PRIMAL!A1" display="RES_CONS_PRIMAL" xr:uid="{A4FFF3BB-1010-4BF1-A0EC-97BC329F98D1}"/>
-    <hyperlink ref="A11" location="Scalar!A1" display="VPROFIT" xr:uid="{29424A31-2A61-44F7-B8E0-D9C8BFA94D6D}"/>
-    <hyperlink ref="A12" location="Scalar!A1" display="VREDCOST" xr:uid="{8A739B92-E010-4D8D-8248-55A7E353228C}"/>
-    <hyperlink ref="A13" location="X!A1" display="X" xr:uid="{F869C5F8-C5C1-4A92-AEAD-B2D89165E018}"/>
-    <hyperlink ref="A14" location="Y!A1" display="Y" xr:uid="{6D1072F0-23B1-4835-BC48-2A5C8DA91D34}"/>
+    <hyperlink ref="A2" location="A!A1" display="A" xr:uid="{EB293F61-3BA2-4CC3-856C-F1C9AF7E70B8}"/>
+    <hyperlink ref="A3" location="b!A1" display="b" xr:uid="{F7C9BA0B-D2D8-4B3C-A4D7-5B4D16147D45}"/>
+    <hyperlink ref="A4" location="c!A1" display="c" xr:uid="{D412A30F-16CA-47BD-9953-114370573CAA}"/>
+    <hyperlink ref="A5" location="plnt!A1" display="plnt" xr:uid="{09978CD7-6C86-40F4-B71F-5A138D253B75}"/>
+    <hyperlink ref="A6" location="Scalar!A1" display="PROFIT_PRIMAL" xr:uid="{9A9482F5-C5D0-4349-AECC-C3A726A096F3}"/>
+    <hyperlink ref="A7" location="Scalar!A1" display="REDCOST_DUAL" xr:uid="{C06EB510-9A1D-456E-A839-32D4C3262B91}"/>
+    <hyperlink ref="A8" location="res!A1" display="res" xr:uid="{1A6D8F10-2050-4232-A35E-CEBA9C79562A}"/>
+    <hyperlink ref="A9" location="RES_CONS_DUAL!A1" display="RES_CONS_DUAL" xr:uid="{B537FEA6-9BE2-415B-A899-87054F8B7981}"/>
+    <hyperlink ref="A10" location="RES_CONS_PRIMAL!A1" display="RES_CONS_PRIMAL" xr:uid="{B9130B72-8C91-407D-9408-CFDD1581DA6E}"/>
+    <hyperlink ref="A11" location="Scalar!A1" display="VPROFIT" xr:uid="{C38A48D0-693C-4076-B7EC-E7FAE4456713}"/>
+    <hyperlink ref="A12" location="Scalar!A1" display="VREDCOST" xr:uid="{2CE72C73-944B-4FDB-8B4F-38BABC982DF4}"/>
+    <hyperlink ref="A13" location="X!A1" display="X" xr:uid="{7242153B-A89C-4C8B-801F-1DF0ED414AA4}"/>
+    <hyperlink ref="A14" location="Y!A1" display="Y" xr:uid="{52785FCF-21A0-4CA2-B7C3-ABA836BA9267}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F233F4C3-32CB-47CD-9986-AAC112F1C3EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264387A5-D1AD-43C1-9BE3-9D73BEFB30F8}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -918,7 +918,7 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>2400</v>
@@ -935,7 +935,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>800</v>
@@ -948,16 +948,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E5" xr:uid="{F233F4C3-32CB-47CD-9986-AAC112F1C3EC}"/>
+  <autoFilter ref="A3:E5" xr:uid="{264387A5-D1AD-43C1-9BE3-9D73BEFB30F8}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{EBADE2B5-EE69-4FBC-9FF9-1AEAB2F0E943}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{0A5D5ECC-1678-4D44-A020-89982902342D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC08AC9-2DD6-46DD-A183-C46308B6D49D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1194DA1A-E4A0-46C0-9BDA-A9C8DDE080AC}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1052,16 +1052,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E6" xr:uid="{CDC08AC9-2DD6-46DD-A183-C46308B6D49D}"/>
+  <autoFilter ref="A3:E6" xr:uid="{1194DA1A-E4A0-46C0-9BDA-A9C8DDE080AC}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{45B32170-DFB7-44D5-9C7F-A308E50B192F}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{02A98083-2655-450D-ACFB-7929992DA705}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526BF3E7-3757-4645-99EB-A7E3D7DAC72B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88C0006-4563-4AF9-9A1F-BAFEC5A972A1}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1206,14 +1206,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{68DE3B7F-5699-44DA-B537-38BD49F72E1A}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{A234E4BA-C68C-4214-BEF4-16177079C1EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419156AA-97A1-444C-8DD8-3ADEED9AC745}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66966E53-41EF-487F-90D5-8ED885A1E833}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1317,16 +1317,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:C9" xr:uid="{419156AA-97A1-444C-8DD8-3ADEED9AC745}"/>
+  <autoFilter ref="A3:C9" xr:uid="{66966E53-41EF-487F-90D5-8ED885A1E833}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{B22EE666-F470-4B36-B79F-5D798FDFD1F5}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{2235FDC7-3A5A-486D-B636-2D9E2E38FFAD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F1FCDD-7C93-49E3-ACC2-8BF8F0A1472D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2723F353-3ED7-4090-BC3C-E35103488DD1}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1385,16 +1385,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:B6" xr:uid="{79F1FCDD-7C93-49E3-ACC2-8BF8F0A1472D}"/>
+  <autoFilter ref="A3:B6" xr:uid="{2723F353-3ED7-4090-BC3C-E35103488DD1}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{985B2F33-A6DE-4577-A348-EEAC48E10959}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{12FA5008-70D9-4F10-9076-95E3ED044FBF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252658C7-B629-43A6-B975-DC4CE189C666}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48A324A2-8F58-458E-85ED-34D864DCF718}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1445,16 +1445,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:B5" xr:uid="{252658C7-B629-43A6-B975-DC4CE189C666}"/>
+  <autoFilter ref="A3:B5" xr:uid="{48A324A2-8F58-458E-85ED-34D864DCF718}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{8FE1DC31-42BE-4991-ADBE-4B6250AAA509}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{90455C30-5A2D-4298-B595-99EA3F888361}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8ACE450-093C-4082-ACBF-3CAC285CFE7A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1917BF81-B106-41E8-8B1E-EA8A6B3717AB}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1496,16 +1496,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:A5" xr:uid="{F8ACE450-093C-4082-ACBF-3CAC285CFE7A}"/>
+  <autoFilter ref="A3:A5" xr:uid="{1917BF81-B106-41E8-8B1E-EA8A6B3717AB}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{91FDF448-C137-4BF1-BB1F-C2BF3FD4A501}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{5A612B21-A4F7-40C0-983D-46C330EBC0B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FACC6F-0D93-4F9B-99B0-9E0FE628B9B1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3452BC93-E6A3-48D4-BF82-ED18DF1E7F7F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1552,16 +1552,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:A6" xr:uid="{15FACC6F-0D93-4F9B-99B0-9E0FE628B9B1}"/>
+  <autoFilter ref="A3:A6" xr:uid="{3452BC93-E6A3-48D4-BF82-ED18DF1E7F7F}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{543DE846-80CE-4E52-BD73-4DC97A4247F3}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{D35C7154-D62A-4C96-ABDE-5D604A77F31A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D255F9E6-7CD5-44F0-AF03-C08D62D2915B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20ECEB7F-D50E-46B1-9FE0-A8D8EA04D123}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1639,16 +1639,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E5" xr:uid="{D255F9E6-7CD5-44F0-AF03-C08D62D2915B}"/>
+  <autoFilter ref="A3:E5" xr:uid="{20ECEB7F-D50E-46B1-9FE0-A8D8EA04D123}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{5712503E-1BC1-4D0E-B246-3C8A1FD50EEB}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{85F28717-E61C-4BE0-B52D-8F2940DE7BE2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{013ED5E4-9385-4342-9886-384DC2C649F9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A259D38-1633-4A3F-8934-3924E6F1C484}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1743,9 +1743,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E6" xr:uid="{013ED5E4-9385-4342-9886-384DC2C649F9}"/>
+  <autoFilter ref="A3:E6" xr:uid="{9A259D38-1633-4A3F-8934-3924E6F1C484}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{69458EF4-AB22-4D79-BB97-516415A4BCB2}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{02546A90-3376-4EEC-B241-41AA3D9A090E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>